<commit_message>
Added stuff in excel
</commit_message>
<xml_diff>
--- a/Presentations/Images/22-10-18/table.xlsx
+++ b/Presentations/Images/22-10-18/table.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="19">
   <si>
     <t xml:space="preserve">TIMIT dataset</t>
   </si>
@@ -52,7 +52,16 @@
     <t xml:space="preserve">'prtscr  :0.08'</t>
   </si>
   <si>
+    <t xml:space="preserve">praat false alarm</t>
+  </si>
+  <si>
     <t xml:space="preserve">Using Original features and Mel filterbank energy with random forest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">praat true detection</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Syll-o-matic true detection</t>
   </si>
   <si>
     <t xml:space="preserve">Using Original features, Mel filterbank energy and VUV features with random forest</t>
@@ -82,6 +91,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -103,12 +113,14 @@
       <color rgb="FF800000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF0000CC"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -257,21 +269,23 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E45"/>
+  <dimension ref="A1:I45"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B40" activeCellId="0" sqref="B40"/>
+      <selection pane="topLeft" activeCell="I11" activeCellId="0" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="69.4642857142857"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.1071428571429"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.5867346938776"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.4744897959184"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="68.5765306122449"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="24.0357142857143"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -363,9 +377,17 @@
         <v>0.901656598472588</v>
       </c>
     </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I8" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
+      </c>
+      <c r="I9" s="0" t="n">
+        <v>0.113554578168733</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -395,6 +417,9 @@
       <c r="E11" s="0" t="n">
         <v>0.861017239230985</v>
       </c>
+      <c r="I11" s="0" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="12" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="4" t="s">
@@ -409,6 +434,9 @@
       <c r="E12" s="4" t="n">
         <v>0.844713790954028</v>
       </c>
+      <c r="I12" s="4" t="n">
+        <v>0.523990403838465</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="0" t="s">
@@ -437,10 +465,18 @@
       <c r="E14" s="0" t="n">
         <v>0.901656598472588</v>
       </c>
+      <c r="I14" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I15" s="0" t="n">
+        <v>0.49640143942423</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="3" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -515,7 +551,7 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -553,7 +589,7 @@
     </row>
     <row r="29" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="4" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C29" s="4" t="n">
         <v>0.16430793937569</v>
@@ -593,9 +629,17 @@
         <v>0.873973404580407</v>
       </c>
     </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I32" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
+      </c>
+      <c r="I33" s="0" t="n">
+        <v>0.182639237330657</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -625,10 +669,13 @@
       <c r="E35" s="0" t="n">
         <v>0.855478006790925</v>
       </c>
+      <c r="I35" s="0" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="36" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="4" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C36" s="4" t="n">
         <v>0.16260162601626</v>
@@ -638,6 +685,9 @@
       </c>
       <c r="E36" s="4" t="n">
         <v>0.846946837424505</v>
+      </c>
+      <c r="I36" s="4" t="n">
+        <v>0.574410436527848</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -667,10 +717,18 @@
       <c r="E38" s="0" t="n">
         <v>0.873973404580407</v>
       </c>
+      <c r="I38" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I39" s="0" t="n">
+        <v>0.476166583040642</v>
+      </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B40" s="3" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -703,7 +761,7 @@
     </row>
     <row r="43" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B43" s="4" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C43" s="4" t="n">
         <v>0.157884171434307</v>

</xml_diff>

<commit_message>
TextGrid files for DTW validation added
</commit_message>
<xml_diff>
--- a/Presentations/Images/22-10-18/table.xlsx
+++ b/Presentations/Images/22-10-18/table.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="21">
   <si>
     <t xml:space="preserve">TIMIT dataset</t>
   </si>
@@ -34,6 +34,12 @@
     <t xml:space="preserve">Overlap</t>
   </si>
   <si>
+    <t xml:space="preserve">New Overlap</t>
+  </si>
+  <si>
+    <t xml:space="preserve">New New Overlap</t>
+  </si>
+  <si>
     <t xml:space="preserve">Using the original 7 features and Random Forest</t>
   </si>
   <si>
@@ -56,9 +62,6 @@
   </si>
   <si>
     <t xml:space="preserve">Using Original features and Mel filterbank energy with random forest</t>
-  </si>
-  <si>
-    <t xml:space="preserve">New Overlap</t>
   </si>
   <si>
     <t xml:space="preserve">praat true detection</t>
@@ -89,7 +92,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -121,6 +124,13 @@
     <font>
       <sz val="10"/>
       <color rgb="FF0000CC"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFCC0000"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -174,7 +184,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -184,6 +194,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -208,7 +222,7 @@
     <indexedColors>
       <rgbColor rgb="FF000000"/>
       <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FFCC0000"/>
       <rgbColor rgb="FF00FF00"/>
       <rgbColor rgb="FF0000CC"/>
       <rgbColor rgb="FFFFFF00"/>
@@ -275,18 +289,21 @@
   <dimension ref="A1:I45"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F31" activeCellId="0" sqref="F31"/>
+      <selection pane="topLeft" activeCell="G29" activeCellId="0" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="67.765306122449"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.0408163265306"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="23.6224489795918"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="66.9540816326531"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.5"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="17.4132653061224"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="6.61224489795918"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="21.8673469387755"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -302,15 +319,21 @@
       <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="3" t="s">
-        <v>4</v>
+      <c r="B2" s="4" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C3" s="0" t="n">
         <v>0.158736505397841</v>
@@ -324,7 +347,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C4" s="0" t="n">
         <v>0.13874450219912</v>
@@ -336,23 +359,23 @@
         <v>0.861017239230985</v>
       </c>
     </row>
-    <row r="5" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="4" t="n">
+    <row r="5" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="5" t="n">
         <v>0.12375049980008</v>
       </c>
-      <c r="D5" s="4" t="n">
+      <c r="D5" s="5" t="n">
         <v>0.221911235505798</v>
       </c>
-      <c r="E5" s="4" t="n">
+      <c r="E5" s="5" t="n">
         <v>0.847244126413872</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="0" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C6" s="0" t="n">
         <v>0.0719712115153939</v>
@@ -366,7 +389,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>0.0331867253098761</v>
@@ -380,15 +403,12 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="I8" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>12</v>
+      <c r="B9" s="4" t="s">
+        <v>13</v>
       </c>
       <c r="I9" s="0" t="n">
         <v>0.113554578168733</v>
@@ -396,7 +416,7 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C10" s="0" t="n">
         <v>0.158736505397841</v>
@@ -410,10 +430,13 @@
       <c r="F10" s="0" t="n">
         <v>0.8542266311</v>
       </c>
+      <c r="G10" s="0" t="n">
+        <v>0.677423197990336</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="0" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>0.13874450219912</v>
@@ -427,33 +450,39 @@
       <c r="F11" s="0" t="n">
         <v>0.8538297009</v>
       </c>
+      <c r="G11" s="0" t="n">
+        <v>0.664567528515489</v>
+      </c>
       <c r="I11" s="0" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="12" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C12" s="4" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B12" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="5" t="n">
         <v>0.128348660535786</v>
       </c>
-      <c r="D12" s="4" t="n">
+      <c r="D12" s="5" t="n">
         <v>0.209916033586565</v>
       </c>
-      <c r="E12" s="4" t="n">
+      <c r="E12" s="5" t="n">
         <v>0.844713790954028</v>
       </c>
-      <c r="F12" s="4" t="n">
+      <c r="F12" s="5" t="n">
         <v>0.8412325806</v>
       </c>
-      <c r="I12" s="4" t="n">
+      <c r="G12" s="5" t="n">
+        <v>0.663716993671487</v>
+      </c>
+      <c r="I12" s="5" t="n">
         <v>0.523990403838465</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="0" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>0.0719712115153939</v>
@@ -467,10 +496,13 @@
       <c r="F13" s="0" t="n">
         <v>0.8589772688</v>
       </c>
+      <c r="G13" s="0" t="n">
+        <v>0.596181219247706</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C14" s="0" t="n">
         <v>0.0331867253098761</v>
@@ -484,8 +516,11 @@
       <c r="F14" s="0" t="n">
         <v>0.8761400346</v>
       </c>
+      <c r="G14" s="0" t="n">
+        <v>0.523946543998182</v>
+      </c>
       <c r="I14" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -494,13 +529,13 @@
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="3" t="s">
-        <v>15</v>
+      <c r="B16" s="4" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>0.158736505397841</v>
@@ -514,7 +549,7 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="0" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C18" s="0" t="n">
         <v>0.13874450219912</v>
@@ -526,23 +561,23 @@
         <v>0.861017239230985</v>
       </c>
     </row>
-    <row r="19" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C19" s="4" t="n">
+    <row r="19" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B19" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" s="5" t="n">
         <v>0.128948420631747</v>
       </c>
-      <c r="D19" s="4" t="n">
+      <c r="D19" s="5" t="n">
         <v>0.208316673330668</v>
       </c>
-      <c r="E19" s="4" t="n">
+      <c r="E19" s="5" t="n">
         <v>0.844031457464541</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="0" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C20" s="0" t="n">
         <v>0.0719712115153939</v>
@@ -556,7 +591,7 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C21" s="0" t="n">
         <v>0.0331867253098761</v>
@@ -570,17 +605,17 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="3" t="s">
-        <v>4</v>
+      <c r="B26" s="4" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C27" s="0" t="n">
         <v>0.156278229448961</v>
@@ -594,10 +629,13 @@
       <c r="F27" s="0" t="n">
         <v>0.852392531990959</v>
       </c>
+      <c r="G27" s="0" t="n">
+        <v>0.700549939828997</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="0" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C28" s="0" t="n">
         <v>0.131687242798354</v>
@@ -611,27 +649,33 @@
       <c r="F28" s="0" t="n">
         <v>0.847177356803191</v>
       </c>
-    </row>
-    <row r="29" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C29" s="4" t="n">
+      <c r="G28" s="0" t="n">
+        <v>0.691457465038471</v>
+      </c>
+    </row>
+    <row r="29" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B29" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C29" s="5" t="n">
         <v>0.16430793937569</v>
       </c>
-      <c r="D29" s="4" t="n">
+      <c r="D29" s="5" t="n">
         <v>0.266686740941483</v>
       </c>
-      <c r="E29" s="4" t="n">
+      <c r="E29" s="5" t="n">
         <v>0.848685526157972</v>
       </c>
-      <c r="F29" s="4" t="n">
+      <c r="F29" s="5" t="n">
         <v>0.834136809073538</v>
+      </c>
+      <c r="G29" s="5" t="n">
+        <v>0.621265359296936</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="0" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C30" s="0" t="n">
         <v>0.0881260664458497</v>
@@ -645,10 +689,13 @@
       <c r="F30" s="0" t="n">
         <v>0.853870806501876</v>
       </c>
+      <c r="G30" s="0" t="n">
+        <v>0.596001986776915</v>
+      </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C31" s="0" t="n">
         <v>0.0752785305630834</v>
@@ -662,15 +709,18 @@
       <c r="F31" s="0" t="n">
         <v>0.847873017000299</v>
       </c>
+      <c r="G31" s="0" t="n">
+        <v>0.56674680377676</v>
+      </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="I32" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B33" s="3" t="s">
-        <v>11</v>
+      <c r="B33" s="4" t="s">
+        <v>13</v>
       </c>
       <c r="I33" s="0" t="n">
         <v>0.182639237330657</v>
@@ -678,7 +728,7 @@
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C34" s="0" t="n">
         <v>0.156278229448961</v>
@@ -692,7 +742,7 @@
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="0" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C35" s="0" t="n">
         <v>0.131687242798354</v>
@@ -704,29 +754,29 @@
         <v>0.855478006790925</v>
       </c>
       <c r="I35" s="0" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="36" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B36" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C36" s="4" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="36" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B36" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C36" s="5" t="n">
         <v>0.16260162601626</v>
       </c>
-      <c r="D36" s="4" t="n">
+      <c r="D36" s="5" t="n">
         <v>0.262671885978119</v>
       </c>
-      <c r="E36" s="4" t="n">
+      <c r="E36" s="5" t="n">
         <v>0.846946837424505</v>
       </c>
-      <c r="I36" s="4" t="n">
+      <c r="I36" s="5" t="n">
         <v>0.574410436527848</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="0" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C37" s="0" t="n">
         <v>0.0881260664458497</v>
@@ -740,7 +790,7 @@
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B38" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C38" s="0" t="n">
         <v>0.0752785305630834</v>
@@ -752,7 +802,7 @@
         <v>0.873973404580407</v>
       </c>
       <c r="I38" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -761,13 +811,13 @@
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B40" s="3" t="s">
-        <v>19</v>
+      <c r="B40" s="4" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B41" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C41" s="0" t="n">
         <v>0.156278229448961</v>
@@ -781,7 +831,7 @@
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B42" s="0" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C42" s="0" t="n">
         <v>0.131687242798354</v>
@@ -793,23 +843,23 @@
         <v>0.855478006790925</v>
       </c>
     </row>
-    <row r="43" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B43" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C43" s="4" t="n">
+    <row r="43" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B43" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C43" s="5" t="n">
         <v>0.157884171434307</v>
       </c>
-      <c r="D43" s="4" t="n">
+      <c r="D43" s="5" t="n">
         <v>0.272106795142026</v>
       </c>
-      <c r="E43" s="4" t="n">
+      <c r="E43" s="5" t="n">
         <v>0.84996401583498</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B44" s="0" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C44" s="0" t="n">
         <v>0.0881260664458497</v>
@@ -823,7 +873,7 @@
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B45" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C45" s="0" t="n">
         <v>0.0752785305630834</v>

</xml_diff>